<commit_message>
Craft Data Init, StartData
</commit_message>
<xml_diff>
--- a/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
+++ b/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Memory\CS-ClickerGame\ClickerGame\Assets\Editor\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766A41FA-1A1A-45BF-B727-F2AB3572556D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB7F9C7-4DF1-441D-9F97-04A49265A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
+    <workbookView xWindow="405" yWindow="3555" windowWidth="26355" windowHeight="11355" activeTab="8" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Doc Rule" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="Upgrade" sheetId="5" r:id="rId6"/>
     <sheet name="Weapon" sheetId="4" r:id="rId7"/>
     <sheet name="Shop" sheetId="3" r:id="rId8"/>
-    <sheet name="String" sheetId="6" r:id="rId9"/>
-    <sheet name="Path" sheetId="7" r:id="rId10"/>
+    <sheet name="StartStatus" sheetId="13" r:id="rId9"/>
+    <sheet name="String" sheetId="6" r:id="rId10"/>
+    <sheet name="Path" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
   <si>
     <t>문서 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,18 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Cost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UpgradeValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CurValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상점</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -370,10 +359,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>__</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Unknown</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -405,6 +390,34 @@
   </si>
   <si>
     <t>Art/Sprite/Upgrade/HealthUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IncreaseStat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InventorySlot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkPower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DefPower</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -892,7 +905,7 @@
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -905,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -927,7 +940,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -938,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -946,7 +959,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -978,7 +991,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1005,6 +1018,115 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD9EE8F-AD06-4E93-BF42-A81103ED372D}">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="35.875" customWidth="1"/>
+    <col min="3" max="3" width="35.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>810001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>810002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>810003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>810004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>810005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>810006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>810007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B661A13C-78C0-4024-AC23-0190BC46D0E0}">
   <dimension ref="A2:C15"/>
   <sheetViews>
@@ -1024,7 +1146,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1035,10 +1157,10 @@
         <v>910001</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1046,10 +1168,10 @@
         <v>910002</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1057,10 +1179,10 @@
         <v>910003</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1068,10 +1190,10 @@
         <v>910004</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1079,10 +1201,10 @@
         <v>910005</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1090,10 +1212,10 @@
         <v>910006</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1101,10 +1223,10 @@
         <v>920001</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1112,10 +1234,10 @@
         <v>930001</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1123,10 +1245,10 @@
         <v>930002</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1134,10 +1256,10 @@
         <v>930003</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1145,10 +1267,10 @@
         <v>940001</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1156,10 +1278,10 @@
         <v>940002</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1167,10 +1289,10 @@
         <v>940003</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1200,75 +1322,75 @@
   <sheetData>
     <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="D7" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1294,31 +1416,31 @@
   <sheetData>
     <row r="1" spans="1:35">
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4">
         <v>44721</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="8">
         <v>1</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U1" s="9">
         <v>2</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="10">
         <v>3</v>
@@ -1327,7 +1449,7 @@
     <row r="2" spans="1:35">
       <c r="B2" s="12">
         <f ca="1">NOW()</f>
-        <v>44724.77381446759</v>
+        <v>44724.816597106481</v>
       </c>
       <c r="F2" s="13">
         <v>6</v>
@@ -1364,16 +1486,16 @@
     </row>
     <row r="3" spans="1:35" ht="16.5" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -1469,7 +1591,7 @@
     <row r="4" spans="1:35">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>_xlfn.IFNA(_xlfn.CONCAT($F$2,"/",MATCH(1,$F4:$AI4)),$E4)</f>
@@ -1503,7 +1625,7 @@
     </row>
     <row r="5" spans="1:35">
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" ref="C5:C20" si="0">_xlfn.IFNA(_xlfn.CONCAT($F$2,"/",MATCH(1,$F5:$AI5)),$E5)</f>
@@ -1529,7 +1651,7 @@
     </row>
     <row r="6" spans="1:35">
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1560,7 +1682,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1594,7 +1716,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1614,7 +1736,7 @@
     </row>
     <row r="9" spans="1:35">
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1634,7 +1756,7 @@
     </row>
     <row r="10" spans="1:35">
       <c r="B10" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1654,7 +1776,7 @@
     </row>
     <row r="11" spans="1:35">
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2103,7 +2225,7 @@
   <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2119,7 +2241,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2144,7 +2266,7 @@
   <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="S1" sqref="S1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2161,19 +2283,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2301,7 +2423,7 @@
         <v>201001</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9">
         <v>930001</v>
@@ -2325,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB62A72-3879-4637-AA7E-A474583661D1}">
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2338,27 +2460,24 @@
     <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>401001</v>
       </c>
@@ -2369,53 +2488,44 @@
         <v>940001</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>5000</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>401002</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>940002</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>10000</v>
       </c>
       <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>401003</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>940003</v>
       </c>
       <c r="D5">
+        <v>2500</v>
+      </c>
+      <c r="E5">
         <v>10</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -2445,7 +2555,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -2550,7 +2660,7 @@
   <dimension ref="A2:G4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2564,22 +2674,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2590,7 +2700,7 @@
         <v>910007</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>399</v>
@@ -2599,7 +2709,7 @@
         <v>4900</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2613,7 +2723,7 @@
         <v>920001</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2622,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <v>1000</v>
@@ -2636,105 +2746,56 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD9EE8F-AD06-4E93-BF42-A81103ED372D}">
-  <dimension ref="A2:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2636E3-D550-4894-8574-537691C76883}">
+  <dimension ref="A2:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="35.875" customWidth="1"/>
-    <col min="3" max="3" width="35.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
-        <v>810001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>810002</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>810003</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>810004</v>
-      </c>
-      <c r="B6" t="s">
+        <v>710001</v>
+      </c>
+      <c r="B3">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>810005</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>810006</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>810007</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Price UI Fix, PlayerSpawn
</commit_message>
<xml_diff>
--- a/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
+++ b/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Memory\CS-ClickerGame\ClickerGame\Assets\Editor\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F630949-2294-4A0C-BCB0-D408E6C05691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C029A960-F484-4FD0-9937-C150AEDCA02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Doc Rule" sheetId="1" r:id="rId1"/>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:AI40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1437,7 +1437,7 @@
     <row r="2" spans="1:35">
       <c r="B2" s="12">
         <f ca="1">NOW()</f>
-        <v>44728.899187384261</v>
+        <v>44729.928234490741</v>
       </c>
       <c r="F2" s="17">
         <v>6</v>
@@ -1621,11 +1621,11 @@
       </c>
       <c r="D5" s="13" t="str">
         <f t="shared" ref="D5:D40" si="2">_xlfn.IFNA(_xlfn.CONCAT($F$2,"/",MATCH($Y$1,$F5:$AI5)),$E5)</f>
-        <v>6/17</v>
+        <v>6/18</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>6/17</v>
+        <v>6/18</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -1639,6 +1639,9 @@
         <v>1</v>
       </c>
       <c r="V5" s="3">
+        <v>2</v>
+      </c>
+      <c r="W5" s="3">
         <v>3</v>
       </c>
     </row>
@@ -2001,15 +2004,15 @@
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>6/16</v>
       </c>
       <c r="D16" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>6/18</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>6/18</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2026,9 +2029,15 @@
       <c r="R16" s="16"/>
       <c r="S16" s="16"/>
       <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
+      <c r="U16" s="16">
+        <v>1</v>
+      </c>
+      <c r="V16" s="16">
+        <v>2</v>
+      </c>
+      <c r="W16" s="16">
+        <v>3</v>
+      </c>
       <c r="X16" s="16"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>

</xml_diff>

<commit_message>
Add Tween, Edit Table, Test Attack
</commit_message>
<xml_diff>
--- a/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
+++ b/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Memory\CS-ClickerGame\ClickerGame\Assets\Editor\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C029A960-F484-4FD0-9937-C150AEDCA02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD3D702-0DC4-4621-9F02-9340330943FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="107">
   <si>
     <t>문서 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -459,11 +459,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IncreasePrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CraftLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkDelay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1391,7 +1399,7 @@
   <dimension ref="A1:AI40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1437,7 +1445,7 @@
     <row r="2" spans="1:35">
       <c r="B2" s="12">
         <f ca="1">NOW()</f>
-        <v>44729.928234490741</v>
+        <v>44730.001048032405</v>
       </c>
       <c r="F2" s="17">
         <v>6</v>
@@ -1638,9 +1646,6 @@
       <c r="U5" s="3">
         <v>1</v>
       </c>
-      <c r="V5" s="3">
-        <v>2</v>
-      </c>
       <c r="W5" s="3">
         <v>3</v>
       </c>
@@ -1812,6 +1817,9 @@
         <v>2</v>
       </c>
       <c r="S10" s="3">
+        <v>2</v>
+      </c>
+      <c r="V10" s="3">
         <v>2</v>
       </c>
       <c r="X10" s="3">
@@ -3212,7 +3220,7 @@
   <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3393,16 +3401,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB62A72-3879-4637-AA7E-A474583661D1}">
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3414,13 +3423,13 @@
         <v>77</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>103</v>
       </c>
       <c r="F2" t="s">
         <v>84</v>
@@ -3428,16 +3437,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>401001</v>
+        <v>401000</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>940001</v>
-      </c>
-      <c r="D3">
-        <v>5000</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -3448,41 +3457,101 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>401002</v>
+        <v>401001</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C4">
-        <v>940002</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>10000</v>
+        <v>940001</v>
       </c>
       <c r="E4">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>401003</v>
+        <v>402000</v>
       </c>
       <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>940002</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>402001</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>940002</v>
+      </c>
+      <c r="E6">
+        <v>11000</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>403000</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C5">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>940003</v>
       </c>
-      <c r="D5">
+      <c r="E7">
         <v>2500</v>
       </c>
-      <c r="E5">
-        <v>5000</v>
-      </c>
-      <c r="F5">
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>403001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>940003</v>
+      </c>
+      <c r="E8">
+        <v>3000</v>
+      </c>
+      <c r="F8">
         <v>10</v>
       </c>
     </row>
@@ -3815,30 +3884,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2636E3-D550-4894-8574-537691C76883}">
-  <dimension ref="A2:H3"/>
+  <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>102</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>87</v>
@@ -3850,21 +3919,27 @@
         <v>29</v>
       </c>
       <c r="H2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
-        <v>710001</v>
+        <v>710000</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>5</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3877,6 +3952,540 @@
       </c>
       <c r="H3">
         <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.2</v>
+      </c>
+      <c r="J3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>710001</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>IF(C3=20,20,SUM(C3,1))</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>150</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>0.2</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>710002</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C19" si="0">IF(C4=20,20,SUM(C4,1))</f>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>0.2</v>
+      </c>
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>710003</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>250</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>0.2</v>
+      </c>
+      <c r="J6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>710004</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>70</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>300</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>710005</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>350</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>0.2</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>710006</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>400</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>0.2</v>
+      </c>
+      <c r="J9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>710007</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>85</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>450</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>0.2</v>
+      </c>
+      <c r="J10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>710008</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>18</v>
+      </c>
+      <c r="G11">
+        <v>500</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <v>0.2</v>
+      </c>
+      <c r="J11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>710009</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>95</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>550</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>0.2</v>
+      </c>
+      <c r="J12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>710010</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>55</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <v>600</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>0.2</v>
+      </c>
+      <c r="J13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>710011</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>105</v>
+      </c>
+      <c r="F14">
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <v>650</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>0.2</v>
+      </c>
+      <c r="J14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>710012</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>65</v>
+      </c>
+      <c r="E15">
+        <v>110</v>
+      </c>
+      <c r="F15">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>700</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>0.2</v>
+      </c>
+      <c r="J15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>710013</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>70</v>
+      </c>
+      <c r="E16">
+        <v>115</v>
+      </c>
+      <c r="F16">
+        <v>28</v>
+      </c>
+      <c r="G16">
+        <v>750</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>0.2</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>710014</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>75</v>
+      </c>
+      <c r="E17">
+        <v>120</v>
+      </c>
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>800</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="I17">
+        <v>0.2</v>
+      </c>
+      <c r="J17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>710015</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <v>125</v>
+      </c>
+      <c r="F18">
+        <v>32</v>
+      </c>
+      <c r="G18">
+        <v>850</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
+      <c r="J18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>710016</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>85</v>
+      </c>
+      <c r="E19">
+        <v>130</v>
+      </c>
+      <c r="F19">
+        <v>34</v>
+      </c>
+      <c r="G19">
+        <v>900</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>0.2</v>
+      </c>
+      <c r="J19">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shop Tab Size Filter, Add Shop Item
</commit_message>
<xml_diff>
--- a/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
+++ b/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Memory\CS-ClickerGame\ClickerGame\Assets\Editor\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF51C8FB-CDB2-485E-9DE7-2D18A23A01E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BAE27E-ABFA-4AC5-8BC4-BCB242FA7DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="3015" windowWidth="19650" windowHeight="12780" firstSheet="1" activeTab="2" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Doc Rule" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3217" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="141">
   <si>
     <t>문서 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -578,14 +578,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Add Gold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>골드 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Art/Sprite/Shop/Coin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -598,6 +590,22 @@
   </si>
   <si>
     <t>광고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골드 추가 10k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Gold 10k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Gold 20k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골드 추가 20k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1379,7 +1387,7 @@
         <v>920002</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1568,7 +1576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC6DBFE-FBAB-4E2A-A711-9A7F0E747B4A}">
   <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
@@ -1616,7 +1624,7 @@
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B2" s="9">
         <f ca="1">NOW()</f>
-        <v>44736.704892939815</v>
+        <v>44737.097659953703</v>
       </c>
       <c r="F2" s="21">
         <v>6</v>
@@ -2577,7 +2585,7 @@
     </row>
     <row r="23" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C23" s="20" t="str">
         <f t="shared" si="4"/>
@@ -75916,10 +75924,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08ADCDD-295A-4117-AF8F-85EFC68CE8EA}">
-  <dimension ref="A2:H3"/>
+  <dimension ref="A2:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -75962,7 +75970,7 @@
         <v>610001</v>
       </c>
       <c r="B3">
-        <v>810007</v>
+        <v>820003</v>
       </c>
       <c r="C3">
         <v>920002</v>
@@ -75981,6 +75989,32 @@
       </c>
       <c r="H3">
         <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>610002</v>
+      </c>
+      <c r="B4">
+        <v>820004</v>
+      </c>
+      <c r="C4">
+        <v>920002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>820002</v>
+      </c>
+      <c r="H4">
+        <v>200000</v>
       </c>
     </row>
   </sheetData>
@@ -76660,10 +76694,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD9EE8F-AD06-4E93-BF42-A81103ED372D}">
-  <dimension ref="A2:C19"/>
+  <dimension ref="A2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -76751,123 +76785,134 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>810007</v>
+        <v>810008</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>810008</v>
+        <v>810009</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>810009</v>
+        <v>810010</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>810010</v>
+        <v>810011</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>810011</v>
+        <v>810012</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>810012</v>
+        <v>810013</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>810013</v>
+        <v>810014</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>810014</v>
+        <v>810015</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>810015</v>
+        <v>820001</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>820001</v>
+        <v>820002</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>820002</v>
+        <v>820003</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>820004</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document Update, StartStatus Rename
</commit_message>
<xml_diff>
--- a/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
+++ b/ClickerGame/Assets/Editor/Data/Excel/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Memory\CS-ClickerGame\ClickerGame\Assets\Editor\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3424DBD9-715C-4FE3-85EE-1ED817430BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2A5F1E-44E4-47BA-8100-08EC49DB0642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21780" yWindow="630" windowWidth="16920" windowHeight="15375" activeTab="2" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
+    <workbookView xWindow="5205" yWindow="390" windowWidth="16920" windowHeight="15375" firstSheet="2" activeTab="7" xr2:uid="{8C878F7F-2353-4352-ABA1-4DA3E9BF44E3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Doc Rule" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Enemy" sheetId="8" r:id="rId5"/>
     <sheet name="Item" sheetId="4" r:id="rId6"/>
     <sheet name="Shop" sheetId="3" r:id="rId7"/>
-    <sheet name="StartStatus" sheetId="13" r:id="rId8"/>
+    <sheet name="Status" sheetId="13" r:id="rId8"/>
     <sheet name="String" sheetId="6" r:id="rId9"/>
     <sheet name="Path" sheetId="7" r:id="rId10"/>
   </sheets>
@@ -1584,7 +1584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC6DBFE-FBAB-4E2A-A711-9A7F0E747B4A}">
   <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
@@ -1632,7 +1632,7 @@
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B2" s="9">
         <f ca="1">NOW()</f>
-        <v>44740.48890196759</v>
+        <v>44741.697821875001</v>
       </c>
       <c r="F2" s="21">
         <v>6</v>
@@ -85108,8 +85108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2636E3-D550-4894-8574-537691C76883}">
   <dimension ref="A2:K203"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="J219" sqref="J219"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>